<commit_message>
debug an application_GUI.py, add env and venv directories to the gitignore
</commit_message>
<xml_diff>
--- a/MSA_data.xlsx
+++ b/MSA_data.xlsx
@@ -22,22 +22,16 @@
     <t>Part</t>
   </si>
   <si>
-    <t>TOP_R201_X</t>
-  </si>
-  <si>
-    <t>TOP_R201_Y</t>
-  </si>
-  <si>
     <t>TOP_R205_X</t>
   </si>
   <si>
     <t>TOP_R205_Y</t>
   </si>
   <si>
-    <t>BOT_R303_X</t>
-  </si>
-  <si>
-    <t>BOT_R303_Y</t>
+    <t>TOP_ R201_X</t>
+  </si>
+  <si>
+    <t>TOP_ R201_Y</t>
   </si>
   <si>
     <t>BOT_R510_X</t>
@@ -46,6 +40,12 @@
     <t>BOT_R510_Y</t>
   </si>
   <si>
+    <t>BOT_ R303_X</t>
+  </si>
+  <si>
+    <t>BOT_ R303_Y</t>
+  </si>
+  <si>
     <t>Desygnator</t>
   </si>
   <si>
@@ -58,16 +58,16 @@
     <t>Tolerancja Y</t>
   </si>
   <si>
-    <t>R201</t>
-  </si>
-  <si>
     <t>R205</t>
   </si>
   <si>
-    <t>R303</t>
+    <t xml:space="preserve"> R201</t>
   </si>
   <si>
     <t>R510</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> R303</t>
   </si>
   <si>
     <t>none</t>
@@ -486,27 +486,15 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.00073</v>
+        <v>0.029464</v>
       </c>
       <c r="D2">
-        <v>5.4E-05</v>
-      </c>
-      <c r="E2">
-        <v>0.029464</v>
-      </c>
-      <c r="F2">
         <v>-0.007656</v>
       </c>
       <c r="G2">
-        <v>-0.008476000000000001</v>
+        <v>-0.003665</v>
       </c>
       <c r="H2">
-        <v>0.005514</v>
-      </c>
-      <c r="I2">
-        <v>-0.003665</v>
-      </c>
-      <c r="J2">
         <v>0.00658</v>
       </c>
       <c r="M2" t="s">
@@ -530,27 +518,15 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.00181</v>
+        <v>0.030259</v>
       </c>
       <c r="D3">
-        <v>-2.3E-05</v>
-      </c>
-      <c r="E3">
-        <v>0.030259</v>
-      </c>
-      <c r="F3">
         <v>-0.008149</v>
       </c>
       <c r="G3">
-        <v>-0.007702</v>
+        <v>-0.001756</v>
       </c>
       <c r="H3">
-        <v>0.006274</v>
-      </c>
-      <c r="I3">
-        <v>-0.001756</v>
-      </c>
-      <c r="J3">
         <v>0.006817999999999999</v>
       </c>
       <c r="M3" t="s">
@@ -574,27 +550,15 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0.002351</v>
+        <v>0.030485</v>
       </c>
       <c r="D4">
-        <v>-0.000244</v>
-      </c>
-      <c r="E4">
-        <v>0.030485</v>
-      </c>
-      <c r="F4">
         <v>-0.007611</v>
       </c>
       <c r="G4">
-        <v>-0.008395</v>
+        <v>-0.002143</v>
       </c>
       <c r="H4">
-        <v>0.007386</v>
-      </c>
-      <c r="I4">
-        <v>-0.002143</v>
-      </c>
-      <c r="J4">
         <v>0.006203999999999999</v>
       </c>
       <c r="M4" t="s">
@@ -618,27 +582,15 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>0.002824</v>
+        <v>0.030628</v>
       </c>
       <c r="D5">
-        <v>0.000183</v>
-      </c>
-      <c r="E5">
-        <v>0.030628</v>
-      </c>
-      <c r="F5">
         <v>-0.007698</v>
       </c>
       <c r="G5">
-        <v>-0.00912</v>
+        <v>-0.003537</v>
       </c>
       <c r="H5">
-        <v>0.00813</v>
-      </c>
-      <c r="I5">
-        <v>-0.003537</v>
-      </c>
-      <c r="J5">
         <v>0.007038</v>
       </c>
       <c r="M5" t="s">
@@ -662,27 +614,15 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>0.003346</v>
+        <v>0.028835</v>
       </c>
       <c r="D6">
-        <v>-0.001105</v>
-      </c>
-      <c r="E6">
-        <v>0.028835</v>
-      </c>
-      <c r="F6">
         <v>-0.008680999999999999</v>
       </c>
       <c r="G6">
-        <v>-0.007962</v>
+        <v>-0.003428</v>
       </c>
       <c r="H6">
-        <v>0.007699</v>
-      </c>
-      <c r="I6">
-        <v>-0.003428</v>
-      </c>
-      <c r="J6">
         <v>0.007076</v>
       </c>
     </row>
@@ -694,27 +634,15 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.003028</v>
+        <v>0.028473</v>
       </c>
       <c r="D7">
-        <v>-0.001068</v>
-      </c>
-      <c r="E7">
-        <v>0.028473</v>
-      </c>
-      <c r="F7">
         <v>-0.006885</v>
       </c>
       <c r="G7">
-        <v>-0.008419000000000001</v>
+        <v>-0.00291</v>
       </c>
       <c r="H7">
-        <v>0.008191</v>
-      </c>
-      <c r="I7">
-        <v>-0.00291</v>
-      </c>
-      <c r="J7">
         <v>0.006867</v>
       </c>
     </row>
@@ -726,27 +654,15 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>0.002836</v>
+        <v>0.02956</v>
       </c>
       <c r="D8">
-        <v>-0.001433</v>
-      </c>
-      <c r="E8">
-        <v>0.02956</v>
-      </c>
-      <c r="F8">
         <v>-0.006881</v>
       </c>
       <c r="G8">
-        <v>-0.008526000000000001</v>
+        <v>-0.002753</v>
       </c>
       <c r="H8">
-        <v>0.008659</v>
-      </c>
-      <c r="I8">
-        <v>-0.002753</v>
-      </c>
-      <c r="J8">
         <v>0.007011999999999999</v>
       </c>
     </row>
@@ -758,27 +674,15 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>0.003227</v>
+        <v>0.029059</v>
       </c>
       <c r="D9">
-        <v>-0.000397</v>
-      </c>
-      <c r="E9">
-        <v>0.029059</v>
-      </c>
-      <c r="F9">
         <v>-0.006898</v>
       </c>
       <c r="G9">
-        <v>-0.008473000000000001</v>
+        <v>-0.002506</v>
       </c>
       <c r="H9">
-        <v>0.009141999999999999</v>
-      </c>
-      <c r="I9">
-        <v>-0.002506</v>
-      </c>
-      <c r="J9">
         <v>0.007176</v>
       </c>
     </row>
@@ -790,27 +694,15 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>0.00385</v>
+        <v>0.028924</v>
       </c>
       <c r="D10">
-        <v>0.001335</v>
-      </c>
-      <c r="E10">
-        <v>0.028924</v>
-      </c>
-      <c r="F10">
         <v>-0.007104</v>
       </c>
       <c r="G10">
-        <v>-0.008074</v>
+        <v>-0.00221</v>
       </c>
       <c r="H10">
-        <v>0.008362</v>
-      </c>
-      <c r="I10">
-        <v>-0.00221</v>
-      </c>
-      <c r="J10">
         <v>0.007371000000000001</v>
       </c>
     </row>
@@ -822,27 +714,15 @@
         <v>2</v>
       </c>
       <c r="C11">
-        <v>0.0278</v>
+        <v>0.021191</v>
       </c>
       <c r="D11">
-        <v>-0.000879</v>
-      </c>
-      <c r="E11">
-        <v>0.021191</v>
-      </c>
-      <c r="F11">
         <v>0.033514</v>
       </c>
       <c r="G11">
-        <v>-0.008666999999999999</v>
+        <v>0.00338</v>
       </c>
       <c r="H11">
-        <v>0.015027</v>
-      </c>
-      <c r="I11">
-        <v>0.00338</v>
-      </c>
-      <c r="J11">
         <v>-0.0006919999999999999</v>
       </c>
     </row>
@@ -854,27 +734,15 @@
         <v>2</v>
       </c>
       <c r="C12">
-        <v>0.028822</v>
+        <v>0.023012</v>
       </c>
       <c r="D12">
-        <v>-0.001658</v>
-      </c>
-      <c r="E12">
-        <v>0.023012</v>
-      </c>
-      <c r="F12">
         <v>0.034405</v>
       </c>
       <c r="G12">
-        <v>-0.008829999999999999</v>
+        <v>0.003698</v>
       </c>
       <c r="H12">
-        <v>0.015019</v>
-      </c>
-      <c r="I12">
-        <v>0.003698</v>
-      </c>
-      <c r="J12">
         <v>-0.000526</v>
       </c>
     </row>
@@ -886,27 +754,15 @@
         <v>2</v>
       </c>
       <c r="C13">
-        <v>0.029746</v>
+        <v>0.022215</v>
       </c>
       <c r="D13">
-        <v>-0.004468</v>
-      </c>
-      <c r="E13">
-        <v>0.022215</v>
-      </c>
-      <c r="F13">
         <v>0.036448</v>
       </c>
       <c r="G13">
-        <v>-0.009468000000000001</v>
+        <v>0.003475</v>
       </c>
       <c r="H13">
-        <v>0.015777</v>
-      </c>
-      <c r="I13">
-        <v>0.003475</v>
-      </c>
-      <c r="J13">
         <v>-0.0008070000000000001</v>
       </c>
     </row>
@@ -918,27 +774,15 @@
         <v>2</v>
       </c>
       <c r="C14">
-        <v>0.028936</v>
+        <v>0.02118</v>
       </c>
       <c r="D14">
-        <v>-0.004288999999999999</v>
-      </c>
-      <c r="E14">
-        <v>0.02118</v>
-      </c>
-      <c r="F14">
         <v>0.033259</v>
       </c>
       <c r="G14">
-        <v>-0.010982</v>
+        <v>0.003772</v>
       </c>
       <c r="H14">
-        <v>0.016486</v>
-      </c>
-      <c r="I14">
-        <v>0.003772</v>
-      </c>
-      <c r="J14">
         <v>-0.000973</v>
       </c>
     </row>
@@ -950,27 +794,15 @@
         <v>2</v>
       </c>
       <c r="C15">
-        <v>0.029017</v>
+        <v>0.020427</v>
       </c>
       <c r="D15">
-        <v>-0.003366</v>
-      </c>
-      <c r="E15">
-        <v>0.020427</v>
-      </c>
-      <c r="F15">
         <v>0.03354099999999999</v>
       </c>
       <c r="G15">
-        <v>-0.010442</v>
+        <v>0.003606</v>
       </c>
       <c r="H15">
-        <v>0.016034</v>
-      </c>
-      <c r="I15">
-        <v>0.003606</v>
-      </c>
-      <c r="J15">
         <v>-0.00109</v>
       </c>
     </row>
@@ -982,31 +814,19 @@
         <v>2</v>
       </c>
       <c r="C16">
-        <v>0.028395</v>
+        <v>0.020857</v>
       </c>
       <c r="D16">
-        <v>-0.003602</v>
-      </c>
-      <c r="E16">
-        <v>0.020857</v>
-      </c>
-      <c r="F16">
         <v>0.036754</v>
       </c>
       <c r="G16">
-        <v>-0.010387</v>
+        <v>0.00387</v>
       </c>
       <c r="H16">
-        <v>0.016467</v>
-      </c>
-      <c r="I16">
-        <v>0.00387</v>
-      </c>
-      <c r="J16">
         <v>-0.000158</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1014,31 +834,19 @@
         <v>2</v>
       </c>
       <c r="C17">
-        <v>0.02943</v>
+        <v>0.020337</v>
       </c>
       <c r="D17">
-        <v>-0.003355</v>
-      </c>
-      <c r="E17">
-        <v>0.020337</v>
-      </c>
-      <c r="F17">
         <v>0.034756</v>
       </c>
       <c r="G17">
-        <v>-0.011193</v>
+        <v>0.003369</v>
       </c>
       <c r="H17">
-        <v>0.015687</v>
-      </c>
-      <c r="I17">
-        <v>0.003369</v>
-      </c>
-      <c r="J17">
         <v>-0.000723</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:8">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1046,31 +854,19 @@
         <v>2</v>
       </c>
       <c r="C18">
-        <v>0.02893</v>
+        <v>0.020281</v>
       </c>
       <c r="D18">
-        <v>-0.003547</v>
-      </c>
-      <c r="E18">
-        <v>0.020281</v>
-      </c>
-      <c r="F18">
         <v>0.036778</v>
       </c>
       <c r="G18">
-        <v>-0.010289</v>
+        <v>0.004787</v>
       </c>
       <c r="H18">
-        <v>0.01575</v>
-      </c>
-      <c r="I18">
-        <v>0.004787</v>
-      </c>
-      <c r="J18">
         <v>7.9E-05</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:8">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1078,31 +874,19 @@
         <v>2</v>
       </c>
       <c r="C19">
-        <v>0.028375</v>
+        <v>0.019621</v>
       </c>
       <c r="D19">
-        <v>-0.003046</v>
-      </c>
-      <c r="E19">
-        <v>0.019621</v>
-      </c>
-      <c r="F19">
         <v>0.03699</v>
       </c>
       <c r="G19">
-        <v>-0.010544</v>
+        <v>0.003863</v>
       </c>
       <c r="H19">
-        <v>0.015498</v>
-      </c>
-      <c r="I19">
-        <v>0.003863</v>
-      </c>
-      <c r="J19">
         <v>0.000505</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:8">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1110,31 +894,19 @@
         <v>3</v>
       </c>
       <c r="C20">
-        <v>0.062163</v>
+        <v>0.028558</v>
       </c>
       <c r="D20">
-        <v>-0.018278</v>
-      </c>
-      <c r="E20">
-        <v>0.028558</v>
-      </c>
-      <c r="F20">
         <v>0.046291</v>
       </c>
       <c r="G20">
-        <v>-0.053388</v>
+        <v>-0.009561</v>
       </c>
       <c r="H20">
-        <v>-0.020517</v>
-      </c>
-      <c r="I20">
-        <v>-0.009561</v>
-      </c>
-      <c r="J20">
         <v>0.029989</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:8">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1142,31 +914,19 @@
         <v>3</v>
       </c>
       <c r="C21">
-        <v>0.063749</v>
+        <v>0.027719</v>
       </c>
       <c r="D21">
-        <v>-0.019301</v>
-      </c>
-      <c r="E21">
-        <v>0.027719</v>
-      </c>
-      <c r="F21">
         <v>0.046227</v>
       </c>
       <c r="G21">
-        <v>-0.052992</v>
+        <v>-0.011079</v>
       </c>
       <c r="H21">
-        <v>-0.020814</v>
-      </c>
-      <c r="I21">
-        <v>-0.011079</v>
-      </c>
-      <c r="J21">
         <v>0.030651</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:8">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1174,31 +934,19 @@
         <v>3</v>
       </c>
       <c r="C22">
-        <v>0.062806</v>
+        <v>0.025943</v>
       </c>
       <c r="D22">
-        <v>-0.018668</v>
-      </c>
-      <c r="E22">
-        <v>0.025943</v>
-      </c>
-      <c r="F22">
         <v>0.046121</v>
       </c>
       <c r="G22">
-        <v>-0.053121</v>
+        <v>-0.009929</v>
       </c>
       <c r="H22">
-        <v>-0.019927</v>
-      </c>
-      <c r="I22">
-        <v>-0.009929</v>
-      </c>
-      <c r="J22">
         <v>0.030348</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:8">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1206,31 +954,19 @@
         <v>3</v>
       </c>
       <c r="C23">
-        <v>0.065125</v>
+        <v>0.026447</v>
       </c>
       <c r="D23">
-        <v>-0.020287</v>
-      </c>
-      <c r="E23">
-        <v>0.026447</v>
-      </c>
-      <c r="F23">
         <v>0.045984</v>
       </c>
       <c r="G23">
-        <v>-0.05376400000000001</v>
+        <v>-0.009186</v>
       </c>
       <c r="H23">
-        <v>-0.019096</v>
-      </c>
-      <c r="I23">
-        <v>-0.009186</v>
-      </c>
-      <c r="J23">
         <v>0.02981</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:8">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1238,31 +974,19 @@
         <v>3</v>
       </c>
       <c r="C24">
-        <v>0.06346</v>
+        <v>0.026198</v>
       </c>
       <c r="D24">
-        <v>-0.019005</v>
-      </c>
-      <c r="E24">
-        <v>0.026198</v>
-      </c>
-      <c r="F24">
         <v>0.046958</v>
       </c>
       <c r="G24">
-        <v>-0.053932</v>
+        <v>-0.009111000000000001</v>
       </c>
       <c r="H24">
-        <v>-0.018739</v>
-      </c>
-      <c r="I24">
-        <v>-0.009111000000000001</v>
-      </c>
-      <c r="J24">
         <v>0.029691</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:8">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1270,31 +994,19 @@
         <v>3</v>
       </c>
       <c r="C25">
-        <v>0.062933</v>
+        <v>0.026253</v>
       </c>
       <c r="D25">
-        <v>-0.019672</v>
-      </c>
-      <c r="E25">
-        <v>0.026253</v>
-      </c>
-      <c r="F25">
         <v>0.046178</v>
       </c>
       <c r="G25">
-        <v>-0.053027</v>
+        <v>-0.011226</v>
       </c>
       <c r="H25">
-        <v>-0.019718</v>
-      </c>
-      <c r="I25">
-        <v>-0.011226</v>
-      </c>
-      <c r="J25">
         <v>0.030118</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:8">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1302,31 +1014,19 @@
         <v>3</v>
       </c>
       <c r="C26">
-        <v>0.063455</v>
+        <v>0.026158</v>
       </c>
       <c r="D26">
-        <v>-0.01848</v>
-      </c>
-      <c r="E26">
-        <v>0.026158</v>
-      </c>
-      <c r="F26">
         <v>0.046699</v>
       </c>
       <c r="G26">
-        <v>-0.05288</v>
+        <v>-0.010968</v>
       </c>
       <c r="H26">
-        <v>-0.020142</v>
-      </c>
-      <c r="I26">
-        <v>-0.010968</v>
-      </c>
-      <c r="J26">
         <v>0.029883</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:8">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1334,31 +1034,19 @@
         <v>3</v>
       </c>
       <c r="C27">
-        <v>0.06336600000000001</v>
+        <v>0.025578</v>
       </c>
       <c r="D27">
-        <v>-0.017805</v>
-      </c>
-      <c r="E27">
-        <v>0.025578</v>
-      </c>
-      <c r="F27">
         <v>0.04634000000000001</v>
       </c>
       <c r="G27">
-        <v>-0.054412</v>
+        <v>-0.010858</v>
       </c>
       <c r="H27">
-        <v>-0.019148</v>
-      </c>
-      <c r="I27">
-        <v>-0.010858</v>
-      </c>
-      <c r="J27">
         <v>0.030419</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:8">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1366,31 +1054,19 @@
         <v>3</v>
       </c>
       <c r="C28">
-        <v>0.063259</v>
+        <v>0.024807</v>
       </c>
       <c r="D28">
-        <v>-0.017136</v>
-      </c>
-      <c r="E28">
-        <v>0.024807</v>
-      </c>
-      <c r="F28">
         <v>0.047852</v>
       </c>
       <c r="G28">
-        <v>-0.05338499999999999</v>
+        <v>-0.01213</v>
       </c>
       <c r="H28">
-        <v>-0.020249</v>
-      </c>
-      <c r="I28">
-        <v>-0.01213</v>
-      </c>
-      <c r="J28">
         <v>0.030405</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:8">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1398,31 +1074,19 @@
         <v>4</v>
       </c>
       <c r="C29">
-        <v>-0.00269</v>
+        <v>0.05319</v>
       </c>
       <c r="D29">
-        <v>-0.072321</v>
-      </c>
-      <c r="E29">
-        <v>0.05319</v>
-      </c>
-      <c r="F29">
         <v>0.004758</v>
       </c>
       <c r="G29">
-        <v>-0.011472</v>
+        <v>-0.005559000000000001</v>
       </c>
       <c r="H29">
-        <v>-0.014472</v>
-      </c>
-      <c r="I29">
-        <v>-0.005559000000000001</v>
-      </c>
-      <c r="J29">
         <v>0.006427</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:8">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1430,31 +1094,19 @@
         <v>4</v>
       </c>
       <c r="C30">
-        <v>-0.002846</v>
+        <v>0.053012</v>
       </c>
       <c r="D30">
-        <v>-0.072274</v>
-      </c>
-      <c r="E30">
-        <v>0.053012</v>
-      </c>
-      <c r="F30">
         <v>0.004549</v>
       </c>
       <c r="G30">
-        <v>-0.010202</v>
+        <v>-0.00304</v>
       </c>
       <c r="H30">
-        <v>-0.015136</v>
-      </c>
-      <c r="I30">
-        <v>-0.00304</v>
-      </c>
-      <c r="J30">
         <v>0.006841</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:8">
       <c r="A31">
         <v>1</v>
       </c>
@@ -1462,31 +1114,19 @@
         <v>4</v>
       </c>
       <c r="C31">
-        <v>-0.001852</v>
+        <v>0.052423</v>
       </c>
       <c r="D31">
-        <v>-0.071823</v>
-      </c>
-      <c r="E31">
-        <v>0.052423</v>
-      </c>
-      <c r="F31">
         <v>0.005573000000000001</v>
       </c>
       <c r="G31">
-        <v>-0.010535</v>
+        <v>-0.002552</v>
       </c>
       <c r="H31">
-        <v>-0.014451</v>
-      </c>
-      <c r="I31">
-        <v>-0.002552</v>
-      </c>
-      <c r="J31">
         <v>0.006408000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:8">
       <c r="A32">
         <v>1</v>
       </c>
@@ -1494,31 +1134,19 @@
         <v>4</v>
       </c>
       <c r="C32">
-        <v>-0.001369</v>
+        <v>0.053869</v>
       </c>
       <c r="D32">
-        <v>-0.07009399999999999</v>
-      </c>
-      <c r="E32">
-        <v>0.053869</v>
-      </c>
-      <c r="F32">
         <v>0.00543</v>
       </c>
       <c r="G32">
-        <v>-0.01041</v>
+        <v>-0.004057000000000001</v>
       </c>
       <c r="H32">
-        <v>-0.014315</v>
-      </c>
-      <c r="I32">
-        <v>-0.004057000000000001</v>
-      </c>
-      <c r="J32">
         <v>0.00595</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:8">
       <c r="A33">
         <v>1</v>
       </c>
@@ -1526,31 +1154,19 @@
         <v>4</v>
       </c>
       <c r="C33">
-        <v>-0.001793</v>
+        <v>0.053378</v>
       </c>
       <c r="D33">
-        <v>-0.071085</v>
-      </c>
-      <c r="E33">
-        <v>0.053378</v>
-      </c>
-      <c r="F33">
         <v>0.00504</v>
       </c>
       <c r="G33">
-        <v>-0.01142</v>
+        <v>-0.003806</v>
       </c>
       <c r="H33">
-        <v>-0.014437</v>
-      </c>
-      <c r="I33">
-        <v>-0.003806</v>
-      </c>
-      <c r="J33">
         <v>0.005905000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:8">
       <c r="A34">
         <v>1</v>
       </c>
@@ -1558,31 +1174,19 @@
         <v>4</v>
       </c>
       <c r="C34">
-        <v>-0.0009559999999999999</v>
+        <v>0.054261</v>
       </c>
       <c r="D34">
-        <v>-0.07178100000000001</v>
-      </c>
-      <c r="E34">
-        <v>0.054261</v>
-      </c>
-      <c r="F34">
         <v>0.006101</v>
       </c>
       <c r="G34">
-        <v>-0.011352</v>
+        <v>-0.003141</v>
       </c>
       <c r="H34">
-        <v>-0.01376</v>
-      </c>
-      <c r="I34">
-        <v>-0.003141</v>
-      </c>
-      <c r="J34">
         <v>0.005777</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:8">
       <c r="A35">
         <v>1</v>
       </c>
@@ -1590,31 +1194,19 @@
         <v>4</v>
       </c>
       <c r="C35">
-        <v>-0.0007099999999999999</v>
+        <v>0.053924</v>
       </c>
       <c r="D35">
-        <v>-0.07162600000000001</v>
-      </c>
-      <c r="E35">
-        <v>0.053924</v>
-      </c>
-      <c r="F35">
         <v>0.006926</v>
       </c>
       <c r="G35">
-        <v>-0.012361</v>
+        <v>-0.002019</v>
       </c>
       <c r="H35">
-        <v>-0.013318</v>
-      </c>
-      <c r="I35">
-        <v>-0.002019</v>
-      </c>
-      <c r="J35">
         <v>0.006508</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:8">
       <c r="A36">
         <v>1</v>
       </c>
@@ -1622,31 +1214,19 @@
         <v>4</v>
       </c>
       <c r="C36">
-        <v>-0.0009379999999999999</v>
+        <v>0.053533</v>
       </c>
       <c r="D36">
-        <v>-0.07123099999999999</v>
-      </c>
-      <c r="E36">
-        <v>0.053533</v>
-      </c>
-      <c r="F36">
         <v>0.006883</v>
       </c>
       <c r="G36">
-        <v>-0.012277</v>
+        <v>-0.002215</v>
       </c>
       <c r="H36">
-        <v>-0.01381</v>
-      </c>
-      <c r="I36">
-        <v>-0.002215</v>
-      </c>
-      <c r="J36">
         <v>0.006753</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:8">
       <c r="A37">
         <v>1</v>
       </c>
@@ -1654,31 +1234,19 @@
         <v>4</v>
       </c>
       <c r="C37">
-        <v>-0.001206</v>
+        <v>0.053231</v>
       </c>
       <c r="D37">
-        <v>-0.07083199999999999</v>
-      </c>
-      <c r="E37">
-        <v>0.053231</v>
-      </c>
-      <c r="F37">
         <v>0.007077</v>
       </c>
       <c r="G37">
-        <v>-0.010591</v>
+        <v>-0.002476</v>
       </c>
       <c r="H37">
-        <v>-0.015304</v>
-      </c>
-      <c r="I37">
-        <v>-0.002476</v>
-      </c>
-      <c r="J37">
         <v>0.00721</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:8">
       <c r="A38">
         <v>1</v>
       </c>
@@ -1686,31 +1254,19 @@
         <v>5</v>
       </c>
       <c r="C38">
-        <v>0.058432</v>
+        <v>0.06250800000000001</v>
       </c>
       <c r="D38">
-        <v>-0.028774</v>
-      </c>
-      <c r="E38">
-        <v>0.06250800000000001</v>
-      </c>
-      <c r="F38">
         <v>0.026183</v>
       </c>
       <c r="G38">
-        <v>-0.028941</v>
+        <v>-0.015024</v>
       </c>
       <c r="H38">
-        <v>-0.038784</v>
-      </c>
-      <c r="I38">
-        <v>-0.015024</v>
-      </c>
-      <c r="J38">
         <v>0.032215</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:8">
       <c r="A39">
         <v>1</v>
       </c>
@@ -1718,31 +1274,19 @@
         <v>5</v>
       </c>
       <c r="C39">
-        <v>0.059327</v>
+        <v>0.061883</v>
       </c>
       <c r="D39">
-        <v>-0.027199</v>
-      </c>
-      <c r="E39">
-        <v>0.061883</v>
-      </c>
-      <c r="F39">
         <v>0.026546</v>
       </c>
       <c r="G39">
-        <v>-0.029097</v>
+        <v>-0.014018</v>
       </c>
       <c r="H39">
-        <v>-0.038493</v>
-      </c>
-      <c r="I39">
-        <v>-0.014018</v>
-      </c>
-      <c r="J39">
         <v>0.032344</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:8">
       <c r="A40">
         <v>1</v>
       </c>
@@ -1750,31 +1294,19 @@
         <v>5</v>
       </c>
       <c r="C40">
-        <v>0.059149</v>
+        <v>0.062138</v>
       </c>
       <c r="D40">
-        <v>-0.028044</v>
-      </c>
-      <c r="E40">
-        <v>0.062138</v>
-      </c>
-      <c r="F40">
         <v>0.026555</v>
       </c>
       <c r="G40">
-        <v>-0.027999</v>
+        <v>-0.014673</v>
       </c>
       <c r="H40">
-        <v>-0.037503</v>
-      </c>
-      <c r="I40">
-        <v>-0.014673</v>
-      </c>
-      <c r="J40">
         <v>0.032668</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:8">
       <c r="A41">
         <v>1</v>
       </c>
@@ -1782,31 +1314,19 @@
         <v>5</v>
       </c>
       <c r="C41">
-        <v>0.059829</v>
+        <v>0.062498</v>
       </c>
       <c r="D41">
-        <v>-0.026647</v>
-      </c>
-      <c r="E41">
-        <v>0.062498</v>
-      </c>
-      <c r="F41">
         <v>0.027074</v>
       </c>
       <c r="G41">
-        <v>-0.027745</v>
+        <v>-0.014898</v>
       </c>
       <c r="H41">
-        <v>-0.03728</v>
-      </c>
-      <c r="I41">
-        <v>-0.014898</v>
-      </c>
-      <c r="J41">
         <v>0.033013</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:8">
       <c r="A42">
         <v>1</v>
       </c>
@@ -1814,31 +1334,19 @@
         <v>5</v>
       </c>
       <c r="C42">
-        <v>0.05943</v>
+        <v>0.062155</v>
       </c>
       <c r="D42">
-        <v>-0.026633</v>
-      </c>
-      <c r="E42">
-        <v>0.062155</v>
-      </c>
-      <c r="F42">
         <v>0.026646</v>
       </c>
       <c r="G42">
-        <v>-0.027886</v>
+        <v>-0.014896</v>
       </c>
       <c r="H42">
-        <v>-0.038131</v>
-      </c>
-      <c r="I42">
-        <v>-0.014896</v>
-      </c>
-      <c r="J42">
         <v>0.03295600000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:8">
       <c r="A43">
         <v>1</v>
       </c>
@@ -1846,31 +1354,19 @@
         <v>5</v>
       </c>
       <c r="C43">
-        <v>0.059048</v>
+        <v>0.062531</v>
       </c>
       <c r="D43">
-        <v>-0.025517</v>
-      </c>
-      <c r="E43">
-        <v>0.062531</v>
-      </c>
-      <c r="F43">
         <v>0.026244</v>
       </c>
       <c r="G43">
-        <v>-0.027954</v>
+        <v>-0.013961</v>
       </c>
       <c r="H43">
-        <v>-0.038578</v>
-      </c>
-      <c r="I43">
-        <v>-0.013961</v>
-      </c>
-      <c r="J43">
         <v>0.032409</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:8">
       <c r="A44">
         <v>1</v>
       </c>
@@ -1878,31 +1374,19 @@
         <v>5</v>
       </c>
       <c r="C44">
-        <v>0.058691</v>
+        <v>0.061939</v>
       </c>
       <c r="D44">
-        <v>-0.027515</v>
-      </c>
-      <c r="E44">
-        <v>0.061939</v>
-      </c>
-      <c r="F44">
         <v>0.026333</v>
       </c>
       <c r="G44">
-        <v>-0.029555</v>
+        <v>-0.012499</v>
       </c>
       <c r="H44">
-        <v>-0.038497</v>
-      </c>
-      <c r="I44">
-        <v>-0.012499</v>
-      </c>
-      <c r="J44">
         <v>0.03285</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:8">
       <c r="A45">
         <v>1</v>
       </c>
@@ -1910,31 +1394,19 @@
         <v>5</v>
       </c>
       <c r="C45">
-        <v>0.058738</v>
+        <v>0.063086</v>
       </c>
       <c r="D45">
-        <v>-0.027473</v>
-      </c>
-      <c r="E45">
-        <v>0.063086</v>
-      </c>
-      <c r="F45">
         <v>0.026457</v>
       </c>
       <c r="G45">
-        <v>-0.029515</v>
+        <v>-0.013386</v>
       </c>
       <c r="H45">
-        <v>-0.038375</v>
-      </c>
-      <c r="I45">
-        <v>-0.013386</v>
-      </c>
-      <c r="J45">
         <v>0.032451</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:8">
       <c r="A46">
         <v>1</v>
       </c>
@@ -1942,27 +1414,15 @@
         <v>5</v>
       </c>
       <c r="C46">
-        <v>0.059725</v>
+        <v>0.061967</v>
       </c>
       <c r="D46">
-        <v>-0.026952</v>
-      </c>
-      <c r="E46">
-        <v>0.061967</v>
-      </c>
-      <c r="F46">
         <v>0.026949</v>
       </c>
       <c r="G46">
-        <v>-0.027112</v>
+        <v>-0.014494</v>
       </c>
       <c r="H46">
-        <v>-0.039165</v>
-      </c>
-      <c r="I46">
-        <v>-0.014494</v>
-      </c>
-      <c r="J46">
         <v>0.032609</v>
       </c>
     </row>

</xml_diff>